<commit_message>
- extended graph with "birds" - added some text - minor clean up
</commit_message>
<xml_diff>
--- a/dist/static/data/sustainable-development-goal-6-1.xlsx
+++ b/dist/static/data/sustainable-development-goal-6-1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrelergier/Documents/Arbeit/Ausbildung/HSLU/4. Semester/03 - Studio Inforamtion Aestehtics/Projekt/hslu-information-aesthetics/static/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA2818C-84D6-244F-9652-A6F740EF2B0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39030DA-FE67-9E47-9EB6-7D4A71E8CB21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="62400" yWindow="-10340" windowWidth="28800" windowHeight="31000" xr2:uid="{561318E5-5228-E347-98E2-3ECFE158814E}"/>
+    <workbookView xWindow="4800" yWindow="460" windowWidth="28800" windowHeight="19620" activeTab="2" xr2:uid="{561318E5-5228-E347-98E2-3ECFE158814E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="45">
   <si>
     <t>GeoAreaName</t>
   </si>
@@ -155,6 +156,12 @@
   </si>
   <si>
     <t>"2005"</t>
+  </si>
+  <si>
+    <t>latest</t>
+  </si>
+  <si>
+    <t>initial</t>
   </si>
 </sst>
 </file>
@@ -544,7 +551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36DA6FB9-0367-5A43-9155-63A607A78E0D}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -985,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A53C32B-AF61-5642-A0AB-385A2F22A647}">
   <dimension ref="A1:V54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="G62" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4485,4 +4492,807 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E70F466-5E42-DD46-9331-09A6155112A2}">
+  <dimension ref="A1:E54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-3.8774299999999968</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1.9529399999999981</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.1158799999999971</v>
+      </c>
+      <c r="D3" s="2">
+        <v>6.7623099999999994</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="2">
+        <v>-0.78724000000001126</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.64677000000000362</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="2">
+        <v>11.987379999999987</v>
+      </c>
+      <c r="D5" s="2">
+        <v>13.653170000000003</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="2">
+        <v>-18.853499999999997</v>
+      </c>
+      <c r="D6" s="2">
+        <v>-23.84149</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="2">
+        <v>-3.9136700000000033</v>
+      </c>
+      <c r="D7" s="2">
+        <v>-11.44894</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="2">
+        <v>-6.7035499999999999</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.33222999999999558</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="2">
+        <v>-9.3222700000000032</v>
+      </c>
+      <c r="D9" s="2">
+        <v>-0.10043000000000291</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="2">
+        <v>-2.5418599999999998</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5.2604299999999995</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2">
+        <v>30.398480000000006</v>
+      </c>
+      <c r="D11" s="2">
+        <v>25.044489999999996</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="2">
+        <v>10.565809999999999</v>
+      </c>
+      <c r="D12" s="2">
+        <v>11.894210000000001</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="2">
+        <v>-51.493369999999999</v>
+      </c>
+      <c r="D13" s="2">
+        <v>-49.537520000000001</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="2">
+        <v>-37.62182</v>
+      </c>
+      <c r="D14" s="2">
+        <v>-44.096000000000004</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="2">
+        <v>-48.479520000000008</v>
+      </c>
+      <c r="D15" s="2">
+        <v>-31.9557</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="2">
+        <v>7.7519999999999953</v>
+      </c>
+      <c r="D16" s="2">
+        <v>8.1869899999999944</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="2">
+        <v>14.315579999999997</v>
+      </c>
+      <c r="D17" s="2">
+        <v>14.30874</v>
+      </c>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="2">
+        <v>28.391030000000001</v>
+      </c>
+      <c r="D18" s="2">
+        <v>22.770619999999994</v>
+      </c>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="2">
+        <v>-35.50526</v>
+      </c>
+      <c r="D19" s="2">
+        <v>-35.78537</v>
+      </c>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="2">
+        <v>-27.656020000000005</v>
+      </c>
+      <c r="D20" s="2">
+        <v>-33.219619999999999</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="2">
+        <v>-22.584240000000008</v>
+      </c>
+      <c r="D21" s="2">
+        <v>-15.847269999999995</v>
+      </c>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="2">
+        <v>-5.025660000000002</v>
+      </c>
+      <c r="D22" s="2">
+        <v>3.6713000000000022</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="2">
+        <v>-6.1727600000000038</v>
+      </c>
+      <c r="D23" s="2">
+        <v>-11.378399999999999</v>
+      </c>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="2">
+        <v>-3.8022400000000118</v>
+      </c>
+      <c r="D24" s="2">
+        <v>-2.8852200000000039</v>
+      </c>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="2">
+        <v>-36.190950000000001</v>
+      </c>
+      <c r="D25" s="2">
+        <v>-35.895060000000001</v>
+      </c>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="2">
+        <v>-21.032970000000002</v>
+      </c>
+      <c r="D26" s="2">
+        <v>-26.877300000000002</v>
+      </c>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="2">
+        <v>-41.153120000000008</v>
+      </c>
+      <c r="D27" s="2">
+        <v>-32.978590000000004</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="2">
+        <v>34.685480000000013</v>
+      </c>
+      <c r="D28" s="2">
+        <v>28.388540000000006</v>
+      </c>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="2">
+        <v>13.434559999999991</v>
+      </c>
+      <c r="D29" s="2">
+        <v>14.497810000000001</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="2">
+        <v>36.36206</v>
+      </c>
+      <c r="D30" s="2">
+        <v>28.675539999999998</v>
+      </c>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="2">
+        <v>5.3767599999999902</v>
+      </c>
+      <c r="D31" s="2">
+        <v>10.982690000000005</v>
+      </c>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="2">
+        <v>14.352680000000007</v>
+      </c>
+      <c r="D32" s="2">
+        <v>9.0427600000000012</v>
+      </c>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="2">
+        <v>-5.4006700000000052</v>
+      </c>
+      <c r="D33" s="2">
+        <v>-11.230130000000003</v>
+      </c>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="2">
+        <v>7.4299999999993815E-2</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1.78904</v>
+      </c>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="2">
+        <v>2.7379799999999932</v>
+      </c>
+      <c r="D35" s="2">
+        <v>-3.2747400000000084</v>
+      </c>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="2">
+        <v>-20.947559999999996</v>
+      </c>
+      <c r="D36" s="2">
+        <v>-11.247720000000001</v>
+      </c>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="2">
+        <v>-8.4196600000000039</v>
+      </c>
+      <c r="D37" s="2">
+        <v>6.8301999999999978</v>
+      </c>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" s="2">
+        <v>-23.159020000000005</v>
+      </c>
+      <c r="D38" s="2">
+        <v>-26.611290000000004</v>
+      </c>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="2">
+        <v>24.750420000000005</v>
+      </c>
+      <c r="D39" s="2">
+        <v>23.387789999999995</v>
+      </c>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="2">
+        <v>-43.083889999999997</v>
+      </c>
+      <c r="D40" s="2">
+        <v>-43.277460000000005</v>
+      </c>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="2">
+        <v>-32.532170000000001</v>
+      </c>
+      <c r="D41" s="2">
+        <v>-40.860570000000003</v>
+      </c>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="2">
+        <v>-43.463670000000008</v>
+      </c>
+      <c r="D42" s="2">
+        <v>-34.638069999999999</v>
+      </c>
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="2">
+        <v>-43.944540000000003</v>
+      </c>
+      <c r="D43" s="2">
+        <v>-46.931629999999998</v>
+      </c>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" s="2">
+        <v>-30.532450000000004</v>
+      </c>
+      <c r="D44" s="2">
+        <v>-37.622900000000001</v>
+      </c>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" s="2">
+        <v>-52.939890000000005</v>
+      </c>
+      <c r="D45" s="2">
+        <v>-51.59187</v>
+      </c>
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" s="2">
+        <v>5.2749400000000009</v>
+      </c>
+      <c r="D46" s="2">
+        <v>5.1101100000000059</v>
+      </c>
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="2">
+        <v>37.206559999999996</v>
+      </c>
+      <c r="D47" s="2">
+        <v>28.35763</v>
+      </c>
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E13:E14 E29 C2:D47">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFEB84"/>
+        <color theme="9"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51:D53">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFC000"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
features: - second graph - styles - text - code restructure
</commit_message>
<xml_diff>
--- a/dist/static/data/sustainable-development-goal-6-1.xlsx
+++ b/dist/static/data/sustainable-development-goal-6-1.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrelergier/Documents/Arbeit/Ausbildung/HSLU/4. Semester/03 - Studio Inforamtion Aestehtics/Projekt/hslu-information-aesthetics/static/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39030DA-FE67-9E47-9EB6-7D4A71E8CB21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133AE9E1-2256-B54A-A6FB-511B7848E450}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="460" windowWidth="28800" windowHeight="19620" activeTab="2" xr2:uid="{561318E5-5228-E347-98E2-3ECFE158814E}"/>
+    <workbookView xWindow="62400" yWindow="-10340" windowWidth="28800" windowHeight="31000" activeTab="3" xr2:uid="{561318E5-5228-E347-98E2-3ECFE158814E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="World" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="117">
   <si>
     <t>GeoAreaName</t>
   </si>
@@ -162,6 +163,222 @@
   </si>
   <si>
     <t>initial</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>"2000"</t>
+  </si>
+  <si>
+    <t>"61.25434"</t>
+  </si>
+  <si>
+    <t>"86.17919"</t>
+  </si>
+  <si>
+    <t>"39.4361"</t>
+  </si>
+  <si>
+    <t>"2001"</t>
+  </si>
+  <si>
+    <t>"61.70454"</t>
+  </si>
+  <si>
+    <t>"86.13555"</t>
+  </si>
+  <si>
+    <t>"39.92612"</t>
+  </si>
+  <si>
+    <t>"86.34688"</t>
+  </si>
+  <si>
+    <t>"62.83692"</t>
+  </si>
+  <si>
+    <t>"41.45364"</t>
+  </si>
+  <si>
+    <t>"2003"</t>
+  </si>
+  <si>
+    <t>"86.29749"</t>
+  </si>
+  <si>
+    <t>"42.55228"</t>
+  </si>
+  <si>
+    <t>"63.60941"</t>
+  </si>
+  <si>
+    <t>"2004"</t>
+  </si>
+  <si>
+    <t>"63.93015"</t>
+  </si>
+  <si>
+    <t>"42.79121"</t>
+  </si>
+  <si>
+    <t>"86.24792"</t>
+  </si>
+  <si>
+    <t>"43.03233"</t>
+  </si>
+  <si>
+    <t>"64.24246"</t>
+  </si>
+  <si>
+    <t>"86.18039"</t>
+  </si>
+  <si>
+    <t>"2006"</t>
+  </si>
+  <si>
+    <t>"86.12835"</t>
+  </si>
+  <si>
+    <t>"43.29615"</t>
+  </si>
+  <si>
+    <t>"64.56688"</t>
+  </si>
+  <si>
+    <t>"2007"</t>
+  </si>
+  <si>
+    <t>"86.07311"</t>
+  </si>
+  <si>
+    <t>"64.88221"</t>
+  </si>
+  <si>
+    <t>"43.55946"</t>
+  </si>
+  <si>
+    <t>"2008"</t>
+  </si>
+  <si>
+    <t>"43.8296"</t>
+  </si>
+  <si>
+    <t>"65.19863"</t>
+  </si>
+  <si>
+    <t>"86.01056"</t>
+  </si>
+  <si>
+    <t>"44.8021"</t>
+  </si>
+  <si>
+    <t>"65.85203"</t>
+  </si>
+  <si>
+    <t>"85.94473"</t>
+  </si>
+  <si>
+    <t>"2010"</t>
+  </si>
+  <si>
+    <t>"85.87328"</t>
+  </si>
+  <si>
+    <t>"66.49626"</t>
+  </si>
+  <si>
+    <t>"45.78517"</t>
+  </si>
+  <si>
+    <t>"2011"</t>
+  </si>
+  <si>
+    <t>"46.81956"</t>
+  </si>
+  <si>
+    <t>"85.77981"</t>
+  </si>
+  <si>
+    <t>"67.12907"</t>
+  </si>
+  <si>
+    <t>"2012"</t>
+  </si>
+  <si>
+    <t>"47.85402"</t>
+  </si>
+  <si>
+    <t>"67.74305"</t>
+  </si>
+  <si>
+    <t>"85.68166"</t>
+  </si>
+  <si>
+    <t>"2013"</t>
+  </si>
+  <si>
+    <t>"48.89293"</t>
+  </si>
+  <si>
+    <t>"68.34628"</t>
+  </si>
+  <si>
+    <t>"85.57937"</t>
+  </si>
+  <si>
+    <t>"2014"</t>
+  </si>
+  <si>
+    <t>"49.93764"</t>
+  </si>
+  <si>
+    <t>"85.4778"</t>
+  </si>
+  <si>
+    <t>"68.94266"</t>
+  </si>
+  <si>
+    <t>"2015"</t>
+  </si>
+  <si>
+    <t>"50.98648"</t>
+  </si>
+  <si>
+    <t>"85.37737"</t>
+  </si>
+  <si>
+    <t>"69.53274"</t>
+  </si>
+  <si>
+    <t>"2016"</t>
+  </si>
+  <si>
+    <t>"85.26961"</t>
+  </si>
+  <si>
+    <t>"52.0242"</t>
+  </si>
+  <si>
+    <t>"70.10356"</t>
+  </si>
+  <si>
+    <t>"2017"</t>
+  </si>
+  <si>
+    <t>"53.03716"</t>
+  </si>
+  <si>
+    <t>"70.64488"</t>
+  </si>
+  <si>
+    <t>"85.14748"</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -4498,7 +4715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E70F466-5E42-DD46-9331-09A6155112A2}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -5295,4 +5512,624 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{705C8AFC-244F-3845-A8E2-300AABC9D512}">
+  <dimension ref="A1:C55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>